<commit_message>
quadratic cost function included
</commit_message>
<xml_diff>
--- a/data/3bus.xlsx
+++ b/data/3bus.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="gen" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,12 +23,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t xml:space="preserve">bus</t>
   </si>
   <si>
-    <t xml:space="preserve">cost</t>
+    <t xml:space="preserve">a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b</t>
   </si>
   <si>
     <t xml:space="preserve">min</t>
@@ -61,6 +64,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -146,10 +150,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -170,18 +174,24 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="n">
-        <v>1</v>
+        <v>0.1</v>
       </c>
       <c r="C2" s="1" t="n">
         <v>10</v>
       </c>
       <c r="D2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="n">
         <v>400</v>
       </c>
     </row>
@@ -190,12 +200,15 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>2</v>
+        <v>0.1</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="D3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
         <v>400</v>
       </c>
     </row>
@@ -218,7 +231,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C25"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -228,16 +241,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -285,7 +298,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -301,7 +314,7 @@
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C25"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,7 +600,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -602,8 +615,8 @@
   </sheetPr>
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:C25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -889,7 +902,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>